<commit_message>
minor updates to excel files
</commit_message>
<xml_diff>
--- a/company_data/sample/VIX INDEX.xlsx
+++ b/company_data/sample/VIX INDEX.xlsx
@@ -9,10 +9,10 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460"/>
+    <workbookView xWindow="4240" yWindow="460" windowWidth="25600" windowHeight="15460"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="VIX Data" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -364,8 +364,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E1503"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView tabSelected="1" topLeftCell="A353" workbookViewId="0">
+      <selection activeCell="F371" sqref="F371"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>